<commit_message>
Some changes in excel file
</commit_message>
<xml_diff>
--- a/data/delete.xlsx
+++ b/data/delete.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Github Repositories\logo-detection\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Github Repositories\voice-controlled-chess\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4DDF75A-0A7E-42A3-A87B-8918DDFE7C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB41B9FC-A27F-4195-9FB8-85CB79DD09A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F60E092F-54B4-4D0E-9906-EE9C3ABEFE83}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Delete this file and add your files here</t>
+    <t>Delete this file and add your files here. Do it asap.</t>
   </si>
 </sst>
 </file>
@@ -381,9 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F439D4D2-6E1B-4394-B4D4-439C25547D40}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>